<commit_message>
Corregir threshold del modelo ganador y actulizar despliegue
</commit_message>
<xml_diff>
--- a/salidas/clasificados.xlsx
+++ b/salidas/clasificados.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="aaP09pHOsDmzn4vJRQxZQ03l/I917uGbNQwI/wzqs/0="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="TLPtOzRwFCJFH0VdL4jJZPF263C9q7PKP5E4dBuasNo="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="5">
   <si>
     <t>ID Paciente</t>
   </si>
@@ -25,6 +25,9 @@
   </si>
   <si>
     <t>Diabetes</t>
+  </si>
+  <si>
+    <t>Normal</t>
   </si>
   <si>
     <t>No ident</t>
@@ -305,8 +308,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.57"/>
-    <col customWidth="1" min="2" max="2" width="16.57"/>
+    <col customWidth="1" min="1" max="1" width="12.43"/>
+    <col customWidth="1" min="2" max="2" width="13.86"/>
     <col customWidth="1" min="3" max="26" width="8.71"/>
   </cols>
   <sheetData>
@@ -379,7 +382,7 @@
         <v>1008.0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
@@ -483,7 +486,7 @@
         <v>1021.0</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
@@ -491,7 +494,7 @@
         <v>1022.0</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
@@ -515,7 +518,7 @@
         <v>1025.0</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
@@ -555,7 +558,7 @@
         <v>1030.0</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
@@ -571,7 +574,7 @@
         <v>1032.0</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
@@ -595,7 +598,7 @@
         <v>1035.0</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
@@ -779,7 +782,7 @@
         <v>1058.0</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
@@ -875,7 +878,7 @@
         <v>1070.0</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72" ht="15.75" customHeight="1">
@@ -1011,7 +1014,7 @@
         <v>1087.0</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89" ht="15.75" customHeight="1">
@@ -1027,7 +1030,7 @@
         <v>1089.0</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91" ht="15.75" customHeight="1">
@@ -1131,7 +1134,7 @@
         <v>1102.0</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="104" ht="15.75" customHeight="1">
@@ -1251,7 +1254,7 @@
         <v>1117.0</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="119" ht="15.75" customHeight="1">
@@ -1355,7 +1358,7 @@
         <v>1130.0</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="132" ht="15.75" customHeight="1">
@@ -1403,7 +1406,7 @@
         <v>1136.0</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="138" ht="15.75" customHeight="1">
@@ -1451,7 +1454,7 @@
         <v>1142.0</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="144" ht="15.75" customHeight="1">
@@ -1523,7 +1526,7 @@
         <v>1151.0</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="153" ht="15.75" customHeight="1">
@@ -1659,7 +1662,7 @@
         <v>1168.0</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="170" ht="15.75" customHeight="1">
@@ -1819,7 +1822,7 @@
         <v>1188.0</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="190" ht="15.75" customHeight="1">
@@ -1827,7 +1830,7 @@
         <v>1189.0</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="191" ht="15.75" customHeight="1">
@@ -1835,7 +1838,7 @@
         <v>1190.0</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="192" ht="15.75" customHeight="1">
@@ -1907,7 +1910,7 @@
         <v>1199.0</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="201" ht="15.75" customHeight="1">
@@ -2035,7 +2038,7 @@
         <v>1215.0</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="217" ht="15.75" customHeight="1">
@@ -2051,7 +2054,7 @@
         <v>1217.0</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="219" ht="15.75" customHeight="1">
@@ -2059,7 +2062,7 @@
         <v>1218.0</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="220" ht="15.75" customHeight="1">
@@ -2259,7 +2262,7 @@
         <v>1243.0</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="245" ht="15.75" customHeight="1">
@@ -2291,7 +2294,7 @@
         <v>1247.0</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="249" ht="15.75" customHeight="1">
@@ -2355,7 +2358,7 @@
         <v>1255.0</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="257" ht="15.75" customHeight="1">
@@ -2371,7 +2374,7 @@
         <v>1257.0</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="259" ht="15.75" customHeight="1">
@@ -2411,7 +2414,7 @@
         <v>1262.0</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="264" ht="15.75" customHeight="1">
@@ -2475,7 +2478,7 @@
         <v>1270.0</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="272" ht="15.75" customHeight="1">
@@ -2515,7 +2518,7 @@
         <v>1275.0</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="277" ht="15.75" customHeight="1">
@@ -2571,7 +2574,7 @@
         <v>1282.0</v>
       </c>
       <c r="B283" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="284" ht="15.75" customHeight="1">
@@ -2579,7 +2582,7 @@
         <v>1283.0</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="285" ht="15.75" customHeight="1">
@@ -2603,7 +2606,7 @@
         <v>1286.0</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="288" ht="15.75" customHeight="1">
@@ -2771,7 +2774,7 @@
         <v>1307.0</v>
       </c>
       <c r="B308" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="309" ht="15.75" customHeight="1">
@@ -2795,7 +2798,7 @@
         <v>1310.0</v>
       </c>
       <c r="B311" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="312" ht="15.75" customHeight="1">
@@ -2899,7 +2902,7 @@
         <v>1323.0</v>
       </c>
       <c r="B324" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="325" ht="15.75" customHeight="1">
@@ -2923,7 +2926,7 @@
         <v>1326.0</v>
       </c>
       <c r="B327" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="328" ht="15.75" customHeight="1">
@@ -3019,7 +3022,7 @@
         <v>1338.0</v>
       </c>
       <c r="B339" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="340" ht="15.75" customHeight="1">
@@ -3067,7 +3070,7 @@
         <v>1344.0</v>
       </c>
       <c r="B345" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="346" ht="15.75" customHeight="1">
@@ -3083,7 +3086,7 @@
         <v>1346.0</v>
       </c>
       <c r="B347" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="348" ht="15.75" customHeight="1">
@@ -3131,7 +3134,7 @@
         <v>1352.0</v>
       </c>
       <c r="B353" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="354" ht="15.75" customHeight="1">
@@ -3219,7 +3222,7 @@
         <v>1363.0</v>
       </c>
       <c r="B364" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="365" ht="15.75" customHeight="1">
@@ -3235,7 +3238,7 @@
         <v>1365.0</v>
       </c>
       <c r="B366" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="367" ht="15.75" customHeight="1">
@@ -3251,7 +3254,7 @@
         <v>1367.0</v>
       </c>
       <c r="B368" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="369" ht="15.75" customHeight="1">
@@ -3419,7 +3422,7 @@
         <v>1388.0</v>
       </c>
       <c r="B389" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="390" ht="15.75" customHeight="1">
@@ -3539,7 +3542,7 @@
         <v>1403.0</v>
       </c>
       <c r="B404" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="405" ht="15.75" customHeight="1">
@@ -3571,7 +3574,7 @@
         <v>1407.0</v>
       </c>
       <c r="B408" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="409" ht="15.75" customHeight="1">
@@ -3603,7 +3606,7 @@
         <v>1411.0</v>
       </c>
       <c r="B412" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="413" ht="15.75" customHeight="1">
@@ -3755,7 +3758,7 @@
         <v>1430.0</v>
       </c>
       <c r="B431" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="432" ht="15.75" customHeight="1">
@@ -4067,7 +4070,7 @@
         <v>1469.0</v>
       </c>
       <c r="B470" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="471" ht="15.75" customHeight="1">
@@ -4107,7 +4110,7 @@
         <v>1474.0</v>
       </c>
       <c r="B475" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="476" ht="15.75" customHeight="1">
@@ -4155,7 +4158,7 @@
         <v>1480.0</v>
       </c>
       <c r="B481" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="482" ht="15.75" customHeight="1">
@@ -4267,7 +4270,7 @@
         <v>1494.0</v>
       </c>
       <c r="B495" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="496" ht="15.75" customHeight="1">
@@ -4459,7 +4462,7 @@
         <v>1518.0</v>
       </c>
       <c r="B519" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="520" ht="15.75" customHeight="1">
@@ -4467,7 +4470,7 @@
         <v>1519.0</v>
       </c>
       <c r="B520" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="521" ht="15.75" customHeight="1">
@@ -4571,7 +4574,7 @@
         <v>1532.0</v>
       </c>
       <c r="B533" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="534" ht="15.75" customHeight="1">
@@ -4603,7 +4606,7 @@
         <v>1536.0</v>
       </c>
       <c r="B537" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="538" ht="15.75" customHeight="1">
@@ -4699,7 +4702,7 @@
         <v>1548.0</v>
       </c>
       <c r="B549" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="550" ht="15.75" customHeight="1">
@@ -4803,7 +4806,7 @@
         <v>1561.0</v>
       </c>
       <c r="B562" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="563" ht="15.75" customHeight="1">
@@ -4939,7 +4942,7 @@
         <v>1578.0</v>
       </c>
       <c r="B579" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="580" ht="15.75" customHeight="1">
@@ -4947,7 +4950,7 @@
         <v>1579.0</v>
       </c>
       <c r="B580" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="581" ht="15.75" customHeight="1">
@@ -4987,7 +4990,7 @@
         <v>1584.0</v>
       </c>
       <c r="B585" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="586" ht="15.75" customHeight="1">
@@ -4995,7 +4998,7 @@
         <v>1585.0</v>
       </c>
       <c r="B586" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="587" ht="15.75" customHeight="1">
@@ -5163,7 +5166,7 @@
         <v>1606.0</v>
       </c>
       <c r="B607" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="608" ht="15.75" customHeight="1">
@@ -5187,7 +5190,7 @@
         <v>1609.0</v>
       </c>
       <c r="B610" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="611" ht="15.75" customHeight="1">
@@ -5363,7 +5366,7 @@
         <v>1631.0</v>
       </c>
       <c r="B632" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="633" ht="15.75" customHeight="1">
@@ -5451,7 +5454,7 @@
         <v>1642.0</v>
       </c>
       <c r="B643" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="644" ht="15.75" customHeight="1">
@@ -5603,7 +5606,7 @@
         <v>1661.0</v>
       </c>
       <c r="B662" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="663" ht="15.75" customHeight="1">
@@ -5715,7 +5718,7 @@
         <v>1675.0</v>
       </c>
       <c r="B676" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="677" ht="15.75" customHeight="1">
@@ -5731,7 +5734,7 @@
         <v>1677.0</v>
       </c>
       <c r="B678" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="679" ht="15.75" customHeight="1">
@@ -5747,7 +5750,7 @@
         <v>1679.0</v>
       </c>
       <c r="B680" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="681" ht="15.75" customHeight="1">
@@ -5787,7 +5790,7 @@
         <v>1684.0</v>
       </c>
       <c r="B685" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="686" ht="15.75" customHeight="1">
@@ -5859,7 +5862,7 @@
         <v>1693.0</v>
       </c>
       <c r="B694" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="695" ht="15.75" customHeight="1">
@@ -5883,7 +5886,7 @@
         <v>1696.0</v>
       </c>
       <c r="B697" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="698" ht="15.75" customHeight="1">
@@ -5931,7 +5934,7 @@
         <v>1702.0</v>
       </c>
       <c r="B703" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="704" ht="15.75" customHeight="1">
@@ -6067,7 +6070,7 @@
         <v>1719.0</v>
       </c>
       <c r="B720" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="721" ht="15.75" customHeight="1">
@@ -6107,7 +6110,7 @@
         <v>1724.0</v>
       </c>
       <c r="B725" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="726" ht="15.75" customHeight="1">
@@ -6115,7 +6118,7 @@
         <v>1725.0</v>
       </c>
       <c r="B726" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="727" ht="15.75" customHeight="1">
@@ -6123,7 +6126,7 @@
         <v>1726.0</v>
       </c>
       <c r="B727" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="728" ht="15.75" customHeight="1">
@@ -6147,7 +6150,7 @@
         <v>1729.0</v>
       </c>
       <c r="B730" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="731" ht="15.75" customHeight="1">
@@ -6323,7 +6326,7 @@
         <v>1751.0</v>
       </c>
       <c r="B752" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="753" ht="15.75" customHeight="1">
@@ -6371,7 +6374,7 @@
         <v>1757.0</v>
       </c>
       <c r="B758" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="759" ht="15.75" customHeight="1">

</xml_diff>